<commit_message>
updated AVCDL mappings and WP.29 R155 spreadsheets based on certification body feedback
</commit_message>
<xml_diff>
--- a/distribution/reference_documents/working_material/UNECE WP.29 R155.xlsx
+++ b/distribution/reference_documents/working_material/UNECE WP.29 R155.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/charles.wilson/Documents/projects/AVCDL/source/reference_documents/working_material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6B1E0C-6123-2E42-995A-1FB9CE2424C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5424685-2F4D-AC4B-A80A-0E42D834BEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21940" yWindow="2440" windowWidth="26840" windowHeight="15940" xr2:uid="{34A2193D-0F67-1544-BFCE-8B57D2CC0421}"/>
+    <workbookView xWindow="16620" yWindow="24120" windowWidth="31360" windowHeight="17940" xr2:uid="{34A2193D-0F67-1544-BFCE-8B57D2CC0421}"/>
   </bookViews>
   <sheets>
-    <sheet name="R155 mitigations" sheetId="1" r:id="rId1"/>
+    <sheet name="R155 attacks" sheetId="2" r:id="rId1"/>
+    <sheet name="R155 attacks (located)" sheetId="3" r:id="rId2"/>
+    <sheet name="R155 mitigations" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +29,7 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="165">
   <si>
     <t>Controls can be found in ISO/SC27/WG5</t>
   </si>
@@ -207,17 +210,335 @@
     <t>mitigation</t>
   </si>
   <si>
-    <t>ID</t>
-  </si>
-  <si>
     <t>area</t>
+  </si>
+  <si>
+    <t>attack</t>
+  </si>
+  <si>
+    <t>Back-end servers used as a means to attack a vehicle or extract data</t>
+  </si>
+  <si>
+    <t>Services from back-end server being disrupted, affecting the operation of a vehicle</t>
+  </si>
+  <si>
+    <t>Vehicle related data held on back-end servers being lost or compromised ("data breach")</t>
+  </si>
+  <si>
+    <t>Spoofing of messages or data received by the vehicle</t>
+  </si>
+  <si>
+    <t>Communication channels used to conduct unauthorized manipulation, deletion or other amendments to vehicle held code/data</t>
+  </si>
+  <si>
+    <t>Communication channels permit untrusted/unreliable messages to be accepted or are vulnerable to session hijacking/replay attacks</t>
+  </si>
+  <si>
+    <t>Denial of service attacks via communication channels to disrupt vehicle functions</t>
+  </si>
+  <si>
+    <t>An unprivileged user is able to gain privileged access to vehicle systems</t>
+  </si>
+  <si>
+    <t>Viruses embedded in communication media are able to infect vehicle systems</t>
+  </si>
+  <si>
+    <t>Misuse or compromise of update procedures</t>
+  </si>
+  <si>
+    <t>It is possible to deny legitimate updates</t>
+  </si>
+  <si>
+    <t>Extraction of vehicle data/code</t>
+  </si>
+  <si>
+    <t>Manipulation of vehicle data/code</t>
+  </si>
+  <si>
+    <t>Erasure of data/code</t>
+  </si>
+  <si>
+    <t>Introduction of malware</t>
+  </si>
+  <si>
+    <t>Introduction of new software or overwrite existing software</t>
+  </si>
+  <si>
+    <t>Disruption of systems or operations</t>
+  </si>
+  <si>
+    <t>Manipulation of vehicle parameters</t>
+  </si>
+  <si>
+    <t>Cryptographic technologies can be compromised or are insufficiently applied</t>
+  </si>
+  <si>
+    <t>Parts or supplies could be compromised to permit vehicles to be attacked</t>
+  </si>
+  <si>
+    <t>Software or hardware development permits vulnerabilities</t>
+  </si>
+  <si>
+    <t>Network design introduces vulnerabilities</t>
+  </si>
+  <si>
+    <t>Unintended transfer of data can occur</t>
+  </si>
+  <si>
+    <t>Physical manipulation of systems can enable an attack</t>
+  </si>
+  <si>
+    <t>Manipulation of the connectivity of vehicle functions enables a cyber-attack</t>
+  </si>
+  <si>
+    <t>this can include telematics; systems that permit remote operations; and systems using short range wireless communications</t>
+  </si>
+  <si>
+    <t>through eavesdropping on communications or through allowing unauthorized access to sensitive files or folders</t>
+  </si>
+  <si>
+    <t>Information can be readily disclosed</t>
+  </si>
+  <si>
+    <t>X2V or diagnostic messages</t>
+  </si>
+  <si>
+    <t>Messages received by the vehicle, or transmitted within it, contain malicious content</t>
+  </si>
+  <si>
+    <t>Hosted third party software</t>
+  </si>
+  <si>
+    <t>entertainment applications, used as a means to attack vehicle systems</t>
+  </si>
+  <si>
+    <t>Devices connected to external interfaces</t>
+  </si>
+  <si>
+    <t>USB ports, OBD port, used as a means to attack vehicle systems</t>
+  </si>
+  <si>
+    <t>Legitimate actors are able to take actions that would unwittingly facilitate a cyber-attack</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Confidentiality</t>
+  </si>
+  <si>
+    <t>Integrity</t>
+  </si>
+  <si>
+    <t>Availability</t>
+  </si>
+  <si>
+    <t>Non-Repudiation</t>
+  </si>
+  <si>
+    <t>Authenticity</t>
+  </si>
+  <si>
+    <t>Accountability</t>
+  </si>
+  <si>
+    <t>Authorization</t>
+  </si>
+  <si>
+    <t>Executables</t>
+  </si>
+  <si>
+    <t>Configuration Data</t>
+  </si>
+  <si>
+    <t>Databases</t>
+  </si>
+  <si>
+    <t>Unstructured Data</t>
+  </si>
+  <si>
+    <t>Credentials</t>
+  </si>
+  <si>
+    <t>Logs</t>
+  </si>
+  <si>
+    <t>PII</t>
+  </si>
+  <si>
+    <t>Packets</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>Layer</t>
+  </si>
+  <si>
+    <t>Physical</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>addressed by attack surface analysis process</t>
+  </si>
+  <si>
+    <t>addressed in normal SDLC processes</t>
+  </si>
+  <si>
+    <t>IT/OT</t>
+  </si>
+  <si>
+    <t>special case of decommissioning / RMA process</t>
+  </si>
+  <si>
+    <t>enforcement of supplier processes</t>
+  </si>
+  <si>
+    <t>all binaries subjected to AV scans (2) prior to code signing</t>
+  </si>
+  <si>
+    <t>addressed by attack surface analysis process / also IT and OT aspects</t>
+  </si>
+  <si>
+    <t>product development has multiple overlapping sets of checks</t>
+  </si>
+  <si>
+    <t>X.1371 ID</t>
+  </si>
+  <si>
+    <t>7.1.2.1</t>
+  </si>
+  <si>
+    <t>7.1.2.4</t>
+  </si>
+  <si>
+    <t>7.1.1.1</t>
+  </si>
+  <si>
+    <t>7.1.1.2</t>
+  </si>
+  <si>
+    <t>7.1.1.3</t>
+  </si>
+  <si>
+    <t>7.1.2.2</t>
+  </si>
+  <si>
+    <t>7.1.2.3</t>
+  </si>
+  <si>
+    <t>7.1.2.5</t>
+  </si>
+  <si>
+    <t>7.1.2.6</t>
+  </si>
+  <si>
+    <t>7.1.2.7</t>
+  </si>
+  <si>
+    <t>7.1.2.8</t>
+  </si>
+  <si>
+    <t>7.1.3.1</t>
+  </si>
+  <si>
+    <t>7.1.3.2</t>
+  </si>
+  <si>
+    <t>7.1.4.1</t>
+  </si>
+  <si>
+    <t>7.1.4.2</t>
+  </si>
+  <si>
+    <t>7.1.5.1</t>
+  </si>
+  <si>
+    <t>R155 ID</t>
+  </si>
+  <si>
+    <t>7.1.5.2</t>
+  </si>
+  <si>
+    <t>7.1.5.3</t>
+  </si>
+  <si>
+    <t>7.2.1.1</t>
+  </si>
+  <si>
+    <t>7.2.1.2</t>
+  </si>
+  <si>
+    <t>7.2.1.3</t>
+  </si>
+  <si>
+    <t>7.2.1.4</t>
+  </si>
+  <si>
+    <t>7.2.1.5</t>
+  </si>
+  <si>
+    <t>7.2.1.6</t>
+  </si>
+  <si>
+    <t>7.2.1.7</t>
+  </si>
+  <si>
+    <t>7.2.2.1</t>
+  </si>
+  <si>
+    <t>7.2.2.2</t>
+  </si>
+  <si>
+    <t>7.2.2.3</t>
+  </si>
+  <si>
+    <t>7.2.2.4</t>
+  </si>
+  <si>
+    <t>7.2.2.5</t>
+  </si>
+  <si>
+    <t>7.2.2.6</t>
+  </si>
+  <si>
+    <t>7.2.2.7</t>
+  </si>
+  <si>
+    <t>not included in R155</t>
+  </si>
+  <si>
+    <t>physical loss of data</t>
+  </si>
+  <si>
+    <t>Misconfiguration of equipment or systems by a legitimate actor</t>
+  </si>
+  <si>
+    <t>Measures shall be implemented for defining and controlling maintenance procedures</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -233,16 +554,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -250,11 +608,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,8 +666,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -579,31 +1031,2048 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F340CB9-5CDC-3740-9735-114BC044CD25}">
-  <dimension ref="A1:F26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F73B16E-1106-7045-9BA1-1A72A4170263}">
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="112.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="106.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
+      <c r="A2" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1"/>
+      <c r="G20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35351D60-5C31-7144-8081-F8728BDB007F}">
+  <dimension ref="A1:Y34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.5" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" customWidth="1"/>
+    <col min="3" max="3" width="112.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="24" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="59.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="D1" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="26" t="s">
+        <v>113</v>
+      </c>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+    </row>
+    <row r="2" spans="1:25" s="2" customFormat="1" ht="102" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>127</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="R2" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="V2" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="W2" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y2" s="16" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="11"/>
+      <c r="W5" s="11"/>
+      <c r="X5" s="11"/>
+      <c r="Y5" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="13"/>
+      <c r="V6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="8"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>133</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="13"/>
+      <c r="V7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="8"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>134</v>
+      </c>
+      <c r="C8" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="13"/>
+      <c r="V8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8" s="8"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="13"/>
+      <c r="V9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y9" s="8"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>135</v>
+      </c>
+      <c r="C10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10" s="13"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="13"/>
+      <c r="L10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" s="1"/>
+      <c r="P10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="8"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>136</v>
+      </c>
+      <c r="C11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="13"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="8"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="8"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>138</v>
+      </c>
+      <c r="C13" t="s">
+        <v>88</v>
+      </c>
+      <c r="D13" s="13"/>
+      <c r="E13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="8"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="8"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>140</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
+      <c r="Y15" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>163</v>
+      </c>
+      <c r="D16" s="23"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="22"/>
+      <c r="M16" s="22"/>
+      <c r="N16" s="22"/>
+      <c r="O16" s="22"/>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="22"/>
+      <c r="S16" s="22"/>
+      <c r="T16" s="22"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="22"/>
+      <c r="W16" s="22"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="18"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="18"/>
+      <c r="L17" s="19"/>
+      <c r="M17" s="19"/>
+      <c r="N17" s="19"/>
+      <c r="O17" s="19"/>
+      <c r="P17" s="19"/>
+      <c r="Q17" s="19"/>
+      <c r="R17" s="19"/>
+      <c r="S17" s="19"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="19"/>
+      <c r="X17" s="19"/>
+      <c r="Y17" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>143</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="18"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="18"/>
+      <c r="L18" s="19"/>
+      <c r="M18" s="19"/>
+      <c r="N18" s="19"/>
+      <c r="O18" s="19"/>
+      <c r="P18" s="19"/>
+      <c r="Q18" s="19"/>
+      <c r="R18" s="19"/>
+      <c r="S18" s="19"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="19"/>
+      <c r="Y18" s="20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="13"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>146</v>
+      </c>
+      <c r="C20" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="13"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="8"/>
+      <c r="T20" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U20" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="13"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K21" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L21" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M21" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" s="14"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="8"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C22" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="13"/>
+      <c r="E22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K22" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y22" s="8"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>149</v>
+      </c>
+      <c r="C23" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="13"/>
+      <c r="E23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y23" s="8"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>150</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="13"/>
+      <c r="E24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" s="8"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>23</v>
+      </c>
+      <c r="B25" t="s">
+        <v>151</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y25" s="8"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>152</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="W26" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="8"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>25</v>
+      </c>
+      <c r="B27" t="s">
+        <v>153</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="13"/>
+      <c r="E27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y27" s="8"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>26</v>
+      </c>
+      <c r="B28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T28" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U28" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="W28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="X28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="8"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>27</v>
+      </c>
+      <c r="B29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19"/>
+      <c r="J29" s="19"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
+      <c r="S29" s="19"/>
+      <c r="T29" s="19"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="19"/>
+      <c r="W29" s="19"/>
+      <c r="X29" s="19"/>
+      <c r="Y29" s="20" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>156</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="18"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+      <c r="Y30" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>29</v>
+      </c>
+      <c r="B31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="18"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="19"/>
+      <c r="Y31" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>158</v>
+      </c>
+      <c r="C32" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="D32" s="23"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="22"/>
+      <c r="N32" s="22"/>
+      <c r="O32" s="22"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="22"/>
+      <c r="R32" s="22"/>
+      <c r="S32" s="22"/>
+      <c r="T32" s="22"/>
+      <c r="U32" s="23"/>
+      <c r="V32" s="22"/>
+      <c r="W32" s="22"/>
+      <c r="X32" s="22"/>
+      <c r="Y32" s="24" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>31</v>
+      </c>
+      <c r="B33" t="s">
+        <v>159</v>
+      </c>
+      <c r="C33" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="L33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>160</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="18"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="K1:S1"/>
+    <mergeCell ref="U1:X1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F340CB9-5CDC-3740-9735-114BC044CD25}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="146.5" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="3.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="59.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="C1" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
+      <c r="C1" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
     </row>
     <row r="2" spans="1:6" s="2" customFormat="1" ht="44" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>57</v>
+      <c r="A2" s="25" t="s">
+        <v>144</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>56</v>
@@ -883,9 +3352,15 @@
       <c r="A19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
+      <c r="B19" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="21" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">

</xml_diff>